<commit_message>
build_DC_4 gives a spot at least
</commit_message>
<xml_diff>
--- a/e_log_excel.xlsx
+++ b/e_log_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Commissioning" sheetId="1" state="visible" r:id="rId2"/>
@@ -1595,9 +1595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1094040</xdr:colOff>
+      <xdr:colOff>1093680</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1611,7 +1611,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1553400" y="10769760"/>
-          <a:ext cx="4426920" cy="3988440"/>
+          <a:ext cx="4426560" cy="3988080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1632,9 +1632,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>462960</xdr:colOff>
+      <xdr:colOff>462600</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1644,7 +1644,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6811920" y="11039760"/>
-          <a:ext cx="2698560" cy="2625120"/>
+          <a:ext cx="2698200" cy="2624760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1700,9 +1700,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2909160</xdr:colOff>
+      <xdr:colOff>2908800</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1712,7 +1712,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9265320" y="11032920"/>
-          <a:ext cx="2691360" cy="2617920"/>
+          <a:ext cx="2691000" cy="2617560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1768,9 +1768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>847080</xdr:colOff>
+      <xdr:colOff>846720</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1784,7 +1784,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="434880" y="6494760"/>
-          <a:ext cx="5298480" cy="3877200"/>
+          <a:ext cx="5298120" cy="3876840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1805,9 +1805,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1733040</xdr:colOff>
+      <xdr:colOff>1732680</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1821,7 +1821,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5999040" y="6313320"/>
-          <a:ext cx="4781520" cy="4114800"/>
+          <a:ext cx="4781160" cy="4114440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1842,9 +1842,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>6725880</xdr:colOff>
+      <xdr:colOff>6725520</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1858,7 +1858,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11004840" y="6098760"/>
-          <a:ext cx="4768560" cy="4363920"/>
+          <a:ext cx="4768200" cy="4363560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1879,9 +1879,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>686880</xdr:colOff>
+      <xdr:colOff>686520</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1895,7 +1895,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16186680" y="5974560"/>
-          <a:ext cx="6579000" cy="6021000"/>
+          <a:ext cx="6578640" cy="6020640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1921,9 +1921,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2497320</xdr:colOff>
+      <xdr:colOff>2496960</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>46080</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1933,7 +1933,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17640" y="4855320"/>
-          <a:ext cx="9420120" cy="1500120"/>
+          <a:ext cx="9427320" cy="1499760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1986,9 +1986,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2968200</xdr:colOff>
+      <xdr:colOff>2967840</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2001,8 +2001,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1548000" y="6608520"/>
-          <a:ext cx="8360640" cy="1396440"/>
+          <a:off x="1549440" y="6608520"/>
+          <a:ext cx="8366400" cy="1396080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2680,7 +2680,7 @@
       <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="50.83"/>
@@ -3774,8 +3774,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4040,7 +4040,7 @@
         <v>0.543055555555555</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>525</v>
+        <v>425</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0" t="s">
@@ -6376,11 +6376,11 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">

</xml_diff>